<commit_message>
consolidation doesn't work at the moment
</commit_message>
<xml_diff>
--- a/exported_data.xlsx
+++ b/exported_data.xlsx
@@ -437,7 +437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -810,6 +810,158 @@
       <c r="B15" t="inlineStr"/>
       <c r="C15" s="5" t="n"/>
     </row>
+    <row r="16">
+      <c r="A16" s="3" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B16" s="3" t="inlineStr">
+        <is>
+          <t>John Doe</t>
+        </is>
+      </c>
+      <c r="C16" s="4" t="inlineStr">
+        <is>
+          <t>Box 5</t>
+        </is>
+      </c>
+      <c r="D16" s="3" t="inlineStr">
+        <is>
+          <t>INCH</t>
+        </is>
+      </c>
+      <c r="E16" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F16" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="G16" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="H16" s="3" t="n">
+        <v>234</v>
+      </c>
+      <c r="I16" s="3">
+        <f>E16*2.54 *F16*2.54 *G16*2.54 /6000</f>
+        <v/>
+      </c>
+      <c r="J16" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K16" s="3">
+        <f>IF(J16="No", 13*MAX(H16,I16), IF(J16="Yes", 14*MAX(H16,I16), "Invalid Input—Yes or No"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>john@gmail.com</t>
+        </is>
+      </c>
+      <c r="C17" s="4" t="inlineStr">
+        <is>
+          <t>Box 6</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>INCH</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>2</v>
+      </c>
+      <c r="F17" t="n">
+        <v>10</v>
+      </c>
+      <c r="G17" t="n">
+        <v>3</v>
+      </c>
+      <c r="H17" t="n">
+        <v>234</v>
+      </c>
+      <c r="I17">
+        <f>E17*2.54 *F17*2.54 *G17*2.54 /6000</f>
+        <v/>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K17">
+        <f>IF(J17="No", 13*MAX(H17,I17), IF(J17="Yes", 14*MAX(H17,I17), "Invalid Input—Yes or No"))</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Cell Number</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>2983748932</t>
+        </is>
+      </c>
+      <c r="C18" s="5" t="n"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Delivery Option</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Door to Door</t>
+        </is>
+      </c>
+      <c r="C19" s="5" t="n"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Wants Insurance</t>
+        </is>
+      </c>
+      <c r="B20" t="b">
+        <v>1</v>
+      </c>
+      <c r="C20" s="5" t="n"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Total Cost</t>
+        </is>
+      </c>
+      <c r="B21">
+        <f>SUM(K16:K17)</f>
+        <v/>
+      </c>
+      <c r="C21" s="5" t="n"/>
+    </row>
+    <row r="22" ht="20" customHeight="1">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" s="5" t="n"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
consolidating boxes in progress
</commit_message>
<xml_diff>
--- a/exported_data.xlsx
+++ b/exported_data.xlsx
@@ -437,7 +437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -810,158 +810,6 @@
       <c r="B15" t="inlineStr"/>
       <c r="C15" s="5" t="n"/>
     </row>
-    <row r="16">
-      <c r="A16" s="3" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B16" s="3" t="inlineStr">
-        <is>
-          <t>John Doe</t>
-        </is>
-      </c>
-      <c r="C16" s="4" t="inlineStr">
-        <is>
-          <t>Box 5</t>
-        </is>
-      </c>
-      <c r="D16" s="3" t="inlineStr">
-        <is>
-          <t>INCH</t>
-        </is>
-      </c>
-      <c r="E16" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="F16" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="G16" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="H16" s="3" t="n">
-        <v>234</v>
-      </c>
-      <c r="I16" s="3">
-        <f>E16*2.54 *F16*2.54 *G16*2.54 /6000</f>
-        <v/>
-      </c>
-      <c r="J16" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="K16" s="3">
-        <f>IF(J16="No", 13*MAX(H16,I16), IF(J16="Yes", 14*MAX(H16,I16), "Invalid Input—Yes or No"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Email</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>john@gmail.com</t>
-        </is>
-      </c>
-      <c r="C17" s="4" t="inlineStr">
-        <is>
-          <t>Box 6</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>INCH</t>
-        </is>
-      </c>
-      <c r="E17" t="n">
-        <v>2</v>
-      </c>
-      <c r="F17" t="n">
-        <v>10</v>
-      </c>
-      <c r="G17" t="n">
-        <v>3</v>
-      </c>
-      <c r="H17" t="n">
-        <v>234</v>
-      </c>
-      <c r="I17">
-        <f>E17*2.54 *F17*2.54 *G17*2.54 /6000</f>
-        <v/>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="K17">
-        <f>IF(J17="No", 13*MAX(H17,I17), IF(J17="Yes", 14*MAX(H17,I17), "Invalid Input—Yes or No"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Cell Number</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>2983748932</t>
-        </is>
-      </c>
-      <c r="C18" s="5" t="n"/>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Delivery Option</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Door to Door</t>
-        </is>
-      </c>
-      <c r="C19" s="5" t="n"/>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Wants Insurance</t>
-        </is>
-      </c>
-      <c r="B20" t="b">
-        <v>1</v>
-      </c>
-      <c r="C20" s="5" t="n"/>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Total Cost</t>
-        </is>
-      </c>
-      <c r="B21">
-        <f>SUM(K16:K17)</f>
-        <v/>
-      </c>
-      <c r="C21" s="5" t="n"/>
-    </row>
-    <row r="22" ht="20" customHeight="1">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Notes</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr"/>
-      <c r="C22" s="5" t="n"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
view order in progress
</commit_message>
<xml_diff>
--- a/exported_data.xlsx
+++ b/exported_data.xlsx
@@ -70,8 +70,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -437,7 +437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -517,15 +517,41 @@
           <t>Justice Oladeji</t>
         </is>
       </c>
-      <c r="C2" s="4" t="n"/>
-      <c r="D2" s="3" t="n"/>
-      <c r="E2" s="3" t="n"/>
-      <c r="F2" s="3" t="n"/>
-      <c r="G2" s="3" t="n"/>
-      <c r="H2" s="3" t="n"/>
-      <c r="I2" s="3" t="n"/>
-      <c r="J2" s="3" t="n"/>
-      <c r="K2" s="3" t="n"/>
+      <c r="C2" s="4" t="inlineStr">
+        <is>
+          <t>Box 1</t>
+        </is>
+      </c>
+      <c r="D2" s="3" t="inlineStr">
+        <is>
+          <t>INCH</t>
+        </is>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="F2" s="3" t="n">
+        <v>33</v>
+      </c>
+      <c r="G2" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="H2" s="3" t="n">
+        <v>7.7</v>
+      </c>
+      <c r="I2" s="3">
+        <f>E2*2.54 *F2*2.54 *G2*2.54 /6000</f>
+        <v/>
+      </c>
+      <c r="J2" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K2" s="3">
+        <f>IF(J2="No", 13*MAX(H2,I2), IF(J2="Yes", 14*MAX(H2,I2), "Invalid Input—Yes or No"))</f>
+        <v/>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -538,7 +564,7 @@
           <t>justice.oladeji@gmail.com</t>
         </is>
       </c>
-      <c r="C3" s="4" t="n"/>
+      <c r="C3" s="5" t="n"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -551,7 +577,7 @@
           <t>4039035399</t>
         </is>
       </c>
-      <c r="C4" s="4" t="n"/>
+      <c r="C4" s="5" t="n"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -564,7 +590,7 @@
           <t>Office to Office</t>
         </is>
       </c>
-      <c r="C5" s="4" t="n"/>
+      <c r="C5" s="5" t="n"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -575,7 +601,7 @@
       <c r="B6" t="b">
         <v>0</v>
       </c>
-      <c r="C6" s="4" t="n"/>
+      <c r="C6" s="5" t="n"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -584,10 +610,10 @@
         </is>
       </c>
       <c r="B7">
-        <f>SUM()</f>
+        <f>SUM(K2:K2)</f>
         <v/>
       </c>
-      <c r="C7" s="4" t="n"/>
+      <c r="C7" s="5" t="n"/>
     </row>
     <row r="8" ht="20" customHeight="1">
       <c r="A8" t="inlineStr">
@@ -596,7 +622,7 @@
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
-      <c r="C8" s="4" t="n"/>
+      <c r="C8" s="5" t="n"/>
     </row>
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
@@ -609,15 +635,41 @@
           <t>Uzoma Emah</t>
         </is>
       </c>
-      <c r="C9" s="4" t="n"/>
-      <c r="D9" s="3" t="n"/>
-      <c r="E9" s="3" t="n"/>
-      <c r="F9" s="3" t="n"/>
-      <c r="G9" s="3" t="n"/>
-      <c r="H9" s="3" t="n"/>
-      <c r="I9" s="3" t="n"/>
-      <c r="J9" s="3" t="n"/>
-      <c r="K9" s="3" t="n"/>
+      <c r="C9" s="4" t="inlineStr">
+        <is>
+          <t>Box 2</t>
+        </is>
+      </c>
+      <c r="D9" s="3" t="inlineStr">
+        <is>
+          <t>INCH</t>
+        </is>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="F9" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="G9" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="H9" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="I9" s="3">
+        <f>E9*2.54 *F9*2.54 *G9*2.54 /6000</f>
+        <v/>
+      </c>
+      <c r="J9" s="3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="K9" s="3">
+        <f>IF(J9="No", 13*MAX(H9,I9), IF(J9="Yes", 14*MAX(H9,I9), "Invalid Input—Yes or No"))</f>
+        <v/>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -630,7 +682,41 @@
           <t>info@ozone-concepts.com</t>
         </is>
       </c>
-      <c r="C10" s="4" t="n"/>
+      <c r="C10" s="4" t="inlineStr">
+        <is>
+          <t>Box 3</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>INCH</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>30</v>
+      </c>
+      <c r="F10" t="n">
+        <v>30</v>
+      </c>
+      <c r="G10" t="n">
+        <v>30</v>
+      </c>
+      <c r="H10" t="n">
+        <v>3</v>
+      </c>
+      <c r="I10">
+        <f>E10*2.54 *F10*2.54 *G10*2.54 /6000</f>
+        <v/>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K10">
+        <f>IF(J10="No", 13*MAX(H10,I10), IF(J10="Yes", 14*MAX(H10,I10), "Invalid Input—Yes or No"))</f>
+        <v/>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -643,7 +729,7 @@
           <t>780-802-4712</t>
         </is>
       </c>
-      <c r="C11" s="4" t="n"/>
+      <c r="C11" s="5" t="n"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -656,7 +742,7 @@
           <t>Door to Door</t>
         </is>
       </c>
-      <c r="C12" s="4" t="n"/>
+      <c r="C12" s="5" t="n"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -667,7 +753,7 @@
       <c r="B13" t="b">
         <v>0</v>
       </c>
-      <c r="C13" s="4" t="n"/>
+      <c r="C13" s="5" t="n"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -676,10 +762,10 @@
         </is>
       </c>
       <c r="B14">
-        <f>SUM()</f>
+        <f>SUM(K9:K10)</f>
         <v/>
       </c>
-      <c r="C14" s="4" t="n"/>
+      <c r="C14" s="5" t="n"/>
     </row>
     <row r="15" ht="20" customHeight="1">
       <c r="A15" t="inlineStr">
@@ -688,217 +774,7 @@
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
-      <c r="C15" s="4" t="n"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="3" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B16" s="3" t="inlineStr">
-        <is>
-          <t>John Doe</t>
-        </is>
-      </c>
-      <c r="C16" s="4" t="n"/>
-      <c r="D16" s="3" t="n"/>
-      <c r="E16" s="3" t="n"/>
-      <c r="F16" s="3" t="n"/>
-      <c r="G16" s="3" t="n"/>
-      <c r="H16" s="3" t="n"/>
-      <c r="I16" s="3" t="n"/>
-      <c r="J16" s="3" t="n"/>
-      <c r="K16" s="3" t="n"/>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Email</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>john@gmail.com</t>
-        </is>
-      </c>
-      <c r="C17" s="4" t="n"/>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Cell Number</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>2983748932</t>
-        </is>
-      </c>
-      <c r="C18" s="4" t="n"/>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Delivery Option</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Door to Door</t>
-        </is>
-      </c>
-      <c r="C19" s="4" t="n"/>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Wants Insurance</t>
-        </is>
-      </c>
-      <c r="B20" t="b">
-        <v>1</v>
-      </c>
-      <c r="C20" s="4" t="n"/>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Total Cost</t>
-        </is>
-      </c>
-      <c r="B21">
-        <f>SUM()</f>
-        <v/>
-      </c>
-      <c r="C21" s="4" t="n"/>
-    </row>
-    <row r="22" ht="20" customHeight="1">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Notes</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr"/>
-      <c r="C22" s="4" t="n"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="3" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B23" s="3" t="inlineStr">
-        <is>
-          <t>Collins Emenike</t>
-        </is>
-      </c>
-      <c r="C23" s="5" t="inlineStr">
-        <is>
-          <t>Box 1</t>
-        </is>
-      </c>
-      <c r="D23" s="3" t="inlineStr">
-        <is>
-          <t>INCH</t>
-        </is>
-      </c>
-      <c r="E23" s="3" t="n">
-        <v>24</v>
-      </c>
-      <c r="F23" s="3" t="n">
-        <v>16</v>
-      </c>
-      <c r="G23" s="3" t="n">
-        <v>13</v>
-      </c>
-      <c r="H23" s="3" t="n">
-        <v>14.5</v>
-      </c>
-      <c r="I23" s="3">
-        <f>E23*2.54 *F23*2.54 *G23*2.54 /6000</f>
-        <v/>
-      </c>
-      <c r="J23" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="K23" s="3">
-        <f>IF(J23="No", 13*MAX(H23,I23), IF(J23="Yes", 14*MAX(H23,I23), "Invalid Input—Yes or No"))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Email</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>collins.emenike@yahoo.com</t>
-        </is>
-      </c>
-      <c r="C24" s="4" t="n"/>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Cell Number</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>not sure</t>
-        </is>
-      </c>
-      <c r="C25" s="4" t="n"/>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Delivery Option</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Office to Office</t>
-        </is>
-      </c>
-      <c r="C26" s="4" t="n"/>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Wants Insurance</t>
-        </is>
-      </c>
-      <c r="B27" t="b">
-        <v>0</v>
-      </c>
-      <c r="C27" s="4" t="n"/>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>Total Cost</t>
-        </is>
-      </c>
-      <c r="B28">
-        <f>SUM(K23:K23)</f>
-        <v/>
-      </c>
-      <c r="C28" s="4" t="n"/>
-    </row>
-    <row r="29" ht="20" customHeight="1">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>Notes</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr"/>
-      <c r="C29" s="4" t="n"/>
+      <c r="C15" s="5" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>